<commit_message>
update get catalog remote service code
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -5,15 +5,17 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/kevinwinarko/eclipse-workspace/DanaPulsaAutomationTest/src/test/java/testCases/otp/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B2CB71B-339A-0640-8948-D1CA482813D7}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B2CD2D-9982-804E-A549-B0473DDADFE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16120" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="2" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="2" r:id="rId1"/>
+    <sheet name="Get Recent Number" sheetId="2" r:id="rId1"/>
+    <sheet name="Get Transaction By ID" sheetId="3" r:id="rId2"/>
+    <sheet name="Get All Catalog" sheetId="4" r:id="rId3"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -33,27 +35,112 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1" uniqueCount="1">
-  <si>
-    <t>id</t>
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+  <si>
+    <t>true</t>
+  </si>
+  <si>
+    <t>9999</t>
+  </si>
+  <si>
+    <t>transactionId</t>
+  </si>
+  <si>
+    <t>userId</t>
+  </si>
+  <si>
+    <t>phonePrefix</t>
+  </si>
+  <si>
+    <t>08773</t>
+  </si>
+  <si>
+    <t>08125</t>
+  </si>
+  <si>
+    <t>08996</t>
+  </si>
+  <si>
+    <t>08565</t>
+  </si>
+  <si>
+    <t>08810</t>
+  </si>
+  <si>
+    <t>08312</t>
+  </si>
+  <si>
+    <t>0812</t>
+  </si>
+  <si>
+    <t>081252</t>
+  </si>
+  <si>
+    <t>02125</t>
+  </si>
+  <si>
+    <t>08ABC</t>
+  </si>
+  <si>
+    <t>081 2</t>
+  </si>
+  <si>
+    <t>+6281</t>
+  </si>
+  <si>
+    <t>description</t>
+  </si>
+  <si>
+    <t>XL</t>
+  </si>
+  <si>
+    <t>Telkomsel</t>
+  </si>
+  <si>
+    <t>Tri</t>
+  </si>
+  <si>
+    <t>Indosat</t>
+  </si>
+  <si>
+    <t>Smartfren</t>
+  </si>
+  <si>
+    <t>Axis</t>
+  </si>
+  <si>
+    <t>Start with +62</t>
+  </si>
+  <si>
+    <t>Start with 62</t>
+  </si>
+  <si>
+    <t>Below 5 characters</t>
+  </si>
+  <si>
+    <t>Exceed 5 characters</t>
+  </si>
+  <si>
+    <t>Undefined provider</t>
+  </si>
+  <si>
+    <t>Not numerical only</t>
+  </si>
+  <si>
+    <t>White space</t>
+  </si>
+  <si>
+    <t>Empty string</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="3" x14ac:knownFonts="1">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
-      <name val="Calibri"/>
-      <family val="2"/>
-      <scheme val="minor"/>
-    </font>
-    <font>
-      <u/>
-      <sz val="12"/>
-      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -66,12 +153,24 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFED7D31"/>
+        <bgColor rgb="FF000000"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="2">
@@ -98,25 +197,24 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="7">
+  <cellXfs count="8">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="1"/>
-    <xf numFmtId="1" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyAlignment="1">
-      <alignment horizontal="left"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="3" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Hyperlink" xfId="1" builtinId="8"/>
+  <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -429,64 +527,206 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09F2C92-1070-F549-ABD8-21E67EECDFEF}">
-  <dimension ref="A1:C12"/>
+  <dimension ref="A1:A4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A11" sqref="A11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5" customWidth="1"/>
-    <col min="2" max="2" width="21.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="14.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="13.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="5" t="s">
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>3</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="5">
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="B2" s="4"/>
-      <c r="C2" s="3"/>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="5"/>
-      <c r="B3" s="2"/>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="5"/>
-      <c r="B4" s="2"/>
-      <c r="C4" s="1"/>
-    </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A5" s="5"/>
-    </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A6" s="5"/>
-    </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A7" s="5"/>
-    </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A8" s="5"/>
-    </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" s="5"/>
-    </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" s="6"/>
-    </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" s="6"/>
-    </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A12" s="5"/>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48440631-96CF-C448-B015-D93981B323AB}">
+  <dimension ref="A1:A4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="A3" sqref="A3"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>2</v>
+      </c>
+    </row>
+    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F7D523-B9EA-2E4C-8630-43530090C6B3}">
+  <dimension ref="A1:B15"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A16" sqref="A16"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="17" style="2" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>4</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>6</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>7</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>8</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>9</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>25</v>
+      </c>
+      <c r="B9" s="6">
+        <v>62812</v>
+      </c>
+    </row>
+    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>26</v>
+      </c>
+      <c r="B10" s="6" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B11" s="6" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B12" s="6" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B13" s="6" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>30</v>
+      </c>
+      <c r="B14" s="6" t="s">
+        <v>15</v>
+      </c>
+    </row>
+    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>31</v>
+      </c>
+      <c r="B15" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update get provider by id code
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -8,14 +8,15 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{58B2CD2D-9982-804E-A549-B0473DDADFE2}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCCAB47-E4FB-9A4F-8043-041C54667EAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="2" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="3" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Recent Number" sheetId="2" r:id="rId1"/>
     <sheet name="Get Transaction By ID" sheetId="3" r:id="rId2"/>
     <sheet name="Get All Catalog" sheetId="4" r:id="rId3"/>
+    <sheet name="Get Provider By ID" sheetId="5" r:id="rId4"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="32">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
   <si>
     <t>true</t>
   </si>
@@ -131,6 +132,36 @@
   </si>
   <si>
     <t>Empty string</t>
+  </si>
+  <si>
+    <t>providerId</t>
+  </si>
+  <si>
+    <t>1</t>
+  </si>
+  <si>
+    <t>2</t>
+  </si>
+  <si>
+    <t>3</t>
+  </si>
+  <si>
+    <t>4</t>
+  </si>
+  <si>
+    <t>5</t>
+  </si>
+  <si>
+    <t>6</t>
+  </si>
+  <si>
+    <t>7</t>
+  </si>
+  <si>
+    <t>Undefined ID</t>
+  </si>
+  <si>
+    <t>Empty String</t>
   </si>
 </sst>
 </file>
@@ -601,8 +632,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F7D523-B9EA-2E4C-8630-43530090C6B3}">
   <dimension ref="A1:B15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A16" sqref="A16"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -731,4 +762,92 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C10451-AC0E-B349-9A91-8F728BB33548}">
+  <dimension ref="A1:B9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="J10" sqref="J10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>32</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B2" s="6" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B3" s="6" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B4" s="6" t="s">
+        <v>35</v>
+      </c>
+    </row>
+    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B5" s="6" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B6" s="6" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B7" s="6" t="s">
+        <v>38</v>
+      </c>
+    </row>
+    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B8" s="6" t="s">
+        <v>39</v>
+      </c>
+    </row>
+    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>41</v>
+      </c>
+      <c r="B9" s="6"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update get payment method name by id code
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -8,15 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1FCCAB47-E4FB-9A4F-8043-041C54667EAF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA2A98F-EB94-4341-8AAF-2BF5CB3D5171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="3" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="4" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Recent Number" sheetId="2" r:id="rId1"/>
     <sheet name="Get Transaction By ID" sheetId="3" r:id="rId2"/>
     <sheet name="Get All Catalog" sheetId="4" r:id="rId3"/>
     <sheet name="Get Provider By ID" sheetId="5" r:id="rId4"/>
+    <sheet name="Get Payment Method Name By ID" sheetId="6" r:id="rId5"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -36,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="51" uniqueCount="42">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
   <si>
     <t>true</t>
   </si>
@@ -162,6 +163,12 @@
   </si>
   <si>
     <t>Empty String</t>
+  </si>
+  <si>
+    <t>methodId</t>
+  </si>
+  <si>
+    <t>Valid ID</t>
   </si>
 </sst>
 </file>
@@ -231,7 +238,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="8">
+  <cellXfs count="10">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -244,6 +251,8 @@
       <alignment horizontal="right"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -561,7 +570,7 @@
   <dimension ref="A1:A4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A11" sqref="A11"/>
+      <selection sqref="A1:A4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -768,7 +777,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C10451-AC0E-B349-9A91-8F728BB33548}">
   <dimension ref="A1:B9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="J10" sqref="J10"/>
     </sheetView>
   </sheetViews>
@@ -850,4 +859,52 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B9D47F-9068-F44D-8E45-59D4A0B7482C}">
+  <dimension ref="A1:B4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B5" sqref="B5"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="8" t="s">
+        <v>17</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>42</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="9" t="s">
+        <v>43</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="9" t="s">
+        <v>40</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>34</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="9" t="s">
+        <v>41</v>
+      </c>
+      <c r="B4" s="4"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
 </file>
</xml_diff>

<commit_message>
update remote service code
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{DCA2A98F-EB94-4341-8AAF-2BF5CB3D5171}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76610D5-44DE-734E-8D92-27B9CAD8C1AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="4" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
@@ -37,7 +37,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="58" uniqueCount="44">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
   <si>
     <t>true</t>
   </si>
@@ -90,9 +90,6 @@
     <t>+6281</t>
   </si>
   <si>
-    <t>description</t>
-  </si>
-  <si>
     <t>XL</t>
   </si>
   <si>
@@ -169,6 +166,39 @@
   </si>
   <si>
     <t>Valid ID</t>
+  </si>
+  <si>
+    <t>testCase</t>
+  </si>
+  <si>
+    <t>51</t>
+  </si>
+  <si>
+    <t>result</t>
+  </si>
+  <si>
+    <t>invalid phone number</t>
+  </si>
+  <si>
+    <t>unknown phone number</t>
+  </si>
+  <si>
+    <t>"id":51</t>
+  </si>
+  <si>
+    <t>unknown transaction</t>
+  </si>
+  <si>
+    <t>invalid request format</t>
+  </si>
+  <si>
+    <t>unknown provider</t>
+  </si>
+  <si>
+    <t>"WALLET"</t>
+  </si>
+  <si>
+    <t>unknown method</t>
   </si>
 </sst>
 </file>
@@ -211,7 +241,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -234,11 +264,24 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color indexed="64"/>
+      </left>
+      <right style="thin">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="10">
+  <cellXfs count="11">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -250,9 +293,10 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="right"/>
     </xf>
-    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -567,34 +611,44 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09F2C92-1070-F549-ABD8-21E67EECDFEF}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:B4"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:A4"/>
-    </sheetView>
+    <sheetView workbookViewId="0"/>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="9" t="s">
         <v>3</v>
       </c>
     </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
+    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
     </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -603,34 +657,59 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48440631-96CF-C448-B015-D93981B323AB}">
-  <dimension ref="A1:A4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3"/>
+      <selection activeCell="F25" sqref="F25"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
         <v>2</v>
       </c>
-    </row>
-    <row r="2" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A2" s="1" t="s">
-        <v>0</v>
-      </c>
-    </row>
-    <row r="3" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A3" s="1" t="s">
+      <c r="C1" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>44</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:1" x14ac:dyDescent="0.2">
-      <c r="A4" s="4"/>
+      <c r="C3" s="8" t="s">
+        <v>49</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -639,134 +718,180 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F7D523-B9EA-2E4C-8630-43530090C6B3}">
-  <dimension ref="A1:B15"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B9"/>
+      <selection activeCell="C1" sqref="C1:C7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="17" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="21" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
-        <v>17</v>
+        <v>43</v>
       </c>
       <c r="B1" s="5" t="s">
         <v>4</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B2" s="6" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B3" s="6" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B4" s="6" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B5" s="6" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B6" s="6" t="s">
         <v>9</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B7" s="6" t="s">
         <v>10</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B8" s="6" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C8" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B9" s="6">
         <v>62812</v>
       </c>
-    </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C9" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B10" s="6" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C10" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B11" s="6" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C11" s="8" t="s">
+        <v>46</v>
+      </c>
+    </row>
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B12" s="6" t="s">
         <v>13</v>
       </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C12" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B13" s="6" t="s">
         <v>14</v>
       </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C13" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B14" s="6" t="s">
         <v>15</v>
       </c>
-    </row>
-    <row r="15" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C14" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="15" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B15" s="6"/>
+      <c r="C15" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -775,86 +900,114 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C10451-AC0E-B349-9A91-8F728BB33548}">
-  <dimension ref="A1:B9"/>
+  <dimension ref="A1:C9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="J10" sqref="J10"/>
+      <selection activeCell="C1" sqref="C1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="5" t="s">
+        <v>31</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="B1" s="5" t="s">
+      <c r="B2" s="6" t="s">
         <v>32</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="4" t="s">
+      <c r="C2" s="8" t="s">
+        <v>17</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
         <v>18</v>
       </c>
-      <c r="B2" s="6" t="s">
+      <c r="B3" s="6" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
+      <c r="C3" s="8" t="s">
+        <v>18</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
         <v>19</v>
       </c>
-      <c r="B3" s="6" t="s">
+      <c r="B4" s="6" t="s">
         <v>34</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="C4" s="8" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>20</v>
       </c>
-      <c r="B4" s="6" t="s">
+      <c r="B5" s="6" t="s">
         <v>35</v>
       </c>
-    </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A5" s="4" t="s">
+      <c r="C5" s="8" t="s">
+        <v>20</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>21</v>
       </c>
-      <c r="B5" s="6" t="s">
+      <c r="B6" s="6" t="s">
         <v>36</v>
       </c>
-    </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A6" s="4" t="s">
+      <c r="C6" s="4" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
         <v>22</v>
       </c>
-      <c r="B6" s="6" t="s">
+      <c r="B7" s="6" t="s">
         <v>37</v>
       </c>
-    </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A7" s="4" t="s">
-        <v>23</v>
-      </c>
-      <c r="B7" s="6" t="s">
+      <c r="C7" s="4" t="s">
+        <v>22</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B8" s="6" t="s">
         <v>38</v>
       </c>
-    </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A8" s="4" t="s">
+      <c r="C8" s="10" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B8" s="6" t="s">
-        <v>39</v>
-      </c>
-    </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A9" s="4" t="s">
-        <v>41</v>
-      </c>
       <c r="B9" s="6"/>
+      <c r="C9" s="10" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -863,46 +1016,59 @@
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B9D47F-9068-F44D-8E45-59D4A0B7482C}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B5" sqref="B5"/>
+      <selection activeCell="C17" sqref="C17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A1" s="8" t="s">
-        <v>17</v>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
         <v>42</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A2" s="9" t="s">
-        <v>43</v>
-      </c>
       <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>52</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
         <v>33</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A3" s="9" t="s">
+      <c r="C3" s="8" t="s">
+        <v>53</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
         <v>40</v>
       </c>
-      <c r="B3" s="1" t="s">
-        <v>34</v>
-      </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="9" t="s">
-        <v>41</v>
-      </c>
       <c r="B4" s="4"/>
+      <c r="C4" s="8" t="s">
+        <v>50</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update code for remote service
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -8,16 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F76610D5-44DE-734E-8D92-27B9CAD8C1AA}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E99BF8-66CD-D646-B0F7-9638813B5ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="4" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="2" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Recent Number" sheetId="2" r:id="rId1"/>
-    <sheet name="Get Transaction By ID" sheetId="3" r:id="rId2"/>
-    <sheet name="Get All Catalog" sheetId="4" r:id="rId3"/>
-    <sheet name="Get Provider By ID" sheetId="5" r:id="rId4"/>
-    <sheet name="Get Payment Method Name By ID" sheetId="6" r:id="rId5"/>
+    <sheet name="Get Transaction By Id By UserId" sheetId="7" r:id="rId2"/>
+    <sheet name="Get Transaction By ID" sheetId="3" r:id="rId3"/>
+    <sheet name="Create Transaction" sheetId="8" r:id="rId4"/>
+    <sheet name="Get All Catalog" sheetId="4" r:id="rId5"/>
+    <sheet name="Get Provider By ID" sheetId="5" r:id="rId6"/>
+    <sheet name="Get Payment Method Name By ID" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -37,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="98" uniqueCount="54">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="83">
   <si>
     <t>true</t>
   </si>
@@ -171,9 +173,6 @@
     <t>testCase</t>
   </si>
   <si>
-    <t>51</t>
-  </si>
-  <si>
     <t>result</t>
   </si>
   <si>
@@ -183,9 +182,6 @@
     <t>unknown phone number</t>
   </si>
   <si>
-    <t>"id":51</t>
-  </si>
-  <si>
     <t>unknown transaction</t>
   </si>
   <si>
@@ -199,6 +195,99 @@
   </si>
   <si>
     <t>unknown method</t>
+  </si>
+  <si>
+    <t>Valid ID (no transaction history)</t>
+  </si>
+  <si>
+    <t>Valid ID (below 10 transaction history)</t>
+  </si>
+  <si>
+    <t>Valid ID (more than 10 transaction history)</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"081252930398","catalog":{"id":13,"provider":{"id":2,"name":"Telkomsel","image":"https://res.cloudinary.com/alvark/image/upload/v1592209103/danapulsa/Telkomsel_Logo_eviigt_nbbrjv.png"},"value":15000,"price":15000}</t>
+  </si>
+  <si>
+    <t>[]</t>
+  </si>
+  <si>
+    <t>"number":"081252930398","provider":{"id":2,"name":"Telkomsel","image":"https://res.cloudinary.com/alvark/image/upload/v1592209103/danapulsa/Telkomsel_Logo_eviigt_nbbrjv.png"}</t>
+  </si>
+  <si>
+    <t>Valid ID (no transaction)</t>
+  </si>
+  <si>
+    <t>Valid ID (with transaction)</t>
+  </si>
+  <si>
+    <t>Undefined user ID</t>
+  </si>
+  <si>
+    <t>Empty String user ID</t>
+  </si>
+  <si>
+    <t>Another user's transaction</t>
+  </si>
+  <si>
+    <t>Undefined transaction ID</t>
+  </si>
+  <si>
+    <t>Empty String transaction ID</t>
+  </si>
+  <si>
+    <t>"method":"WALLET","phoneNumber":"081252930398","catalog":{"id":13,"provider":{"id":2,"name":"Telkomsel","image":"https://res.cloudinary.com/alvark/image/upload/v1592209103/danapulsa/Telkomsel_Logo_eviigt_nbbrjv.png"},"value":15000,"price":15000}</t>
+  </si>
+  <si>
+    <t>phoneNumber</t>
+  </si>
+  <si>
+    <t>catalogId</t>
+  </si>
+  <si>
+    <t>081252930398</t>
+  </si>
+  <si>
+    <t>Below 9 characters</t>
+  </si>
+  <si>
+    <t>Exceed 13 characters</t>
+  </si>
+  <si>
+    <t>+628125293039</t>
+  </si>
+  <si>
+    <t>6281252930398</t>
+  </si>
+  <si>
+    <t>08125293</t>
+  </si>
+  <si>
+    <t>08125293039812</t>
+  </si>
+  <si>
+    <t>021252930398</t>
+  </si>
+  <si>
+    <t>081252930ABC</t>
+  </si>
+  <si>
+    <t>081 252930398</t>
+  </si>
+  <si>
+    <t>Different provider</t>
+  </si>
+  <si>
+    <t>Empty string phone number</t>
+  </si>
+  <si>
+    <t>Undefined catalog ID</t>
+  </si>
+  <si>
+    <t>Empty String catalog ID</t>
+  </si>
+  <si>
+    <t>"number":"081252161795","provider":{"id":2,"name":"Telkomsel","image":"https://res.cloudinary.com/alvark/image/upload/v1592209103/danapulsa/Telkomsel_Logo_eviigt_nbbrjv.png"}</t>
   </si>
 </sst>
 </file>
@@ -241,7 +330,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="3">
+  <borders count="2">
     <border>
       <left/>
       <right/>
@@ -264,19 +353,6 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color indexed="64"/>
-      </left>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -295,8 +371,8 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
-    <xf numFmtId="49" fontId="1" fillId="2" borderId="2" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -611,44 +687,81 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A09F2C92-1070-F549-ABD8-21E67EECDFEF}">
-  <dimension ref="A1:B4"/>
+  <dimension ref="A1:C6"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="C13" sqref="C13"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="26.5" style="2" customWidth="1"/>
+    <col min="1" max="1" width="36.6640625" style="2" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="159.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="3" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>52</v>
       </c>
       <c r="B2" s="1" t="s">
         <v>0</v>
       </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="C2" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
+        <v>53</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>57</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>54</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="8" t="s">
+        <v>82</v>
+      </c>
+    </row>
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
         <v>39</v>
       </c>
-      <c r="B3" s="1" t="s">
+      <c r="B5" s="1" t="s">
         <v>1</v>
       </c>
-    </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
+      <c r="C5" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
         <v>40</v>
       </c>
-      <c r="B4" s="4"/>
+      <c r="B6" s="4"/>
+      <c r="C6" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -656,59 +769,125 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48440631-96CF-C448-B015-D93981B323AB}">
-  <dimension ref="A1:C4"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2C1876-3DA3-8644-B3D6-CD5FFA8B91C1}">
+  <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="F25" sqref="F25"/>
+      <selection activeCell="D29" sqref="D29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="23.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="223.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" s="7" t="s">
         <v>43</v>
       </c>
       <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
         <v>2</v>
       </c>
-      <c r="C1" s="7" t="s">
-        <v>45</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="D1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="4" t="s">
-        <v>42</v>
+        <v>58</v>
       </c>
       <c r="B2" s="1" t="s">
-        <v>44</v>
-      </c>
-      <c r="C2" s="8" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8" t="s">
         <v>48</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="4" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="1" t="s">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
         <v>1</v>
       </c>
-      <c r="C3" s="8" t="s">
-        <v>49</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="4" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="8" t="s">
-        <v>50</v>
+      <c r="D6" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>47</v>
       </c>
     </row>
   </sheetData>
@@ -717,11 +896,385 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48440631-96CF-C448-B015-D93981B323AB}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="C34" sqref="C34"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="205.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="4" t="s">
+        <v>55</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A5EF4B-A648-C44F-8302-8A78460D835D}">
+  <dimension ref="A1:E20"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="G18" sqref="G18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="24.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>67</v>
+      </c>
+      <c r="E1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="6" t="s">
+        <v>5</v>
+      </c>
+      <c r="D2" s="8">
+        <v>1</v>
+      </c>
+      <c r="E2" s="8"/>
+    </row>
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>18</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D3" s="8">
+        <v>13</v>
+      </c>
+      <c r="E3" s="8"/>
+    </row>
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>19</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="6" t="s">
+        <v>7</v>
+      </c>
+      <c r="D4" s="8">
+        <v>26</v>
+      </c>
+      <c r="E4" s="8"/>
+    </row>
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>20</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="6" t="s">
+        <v>8</v>
+      </c>
+      <c r="D5" s="8">
+        <v>44</v>
+      </c>
+      <c r="E5" s="8"/>
+    </row>
+    <row r="6" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>21</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="D6" s="8">
+        <v>58</v>
+      </c>
+      <c r="E6" s="4"/>
+    </row>
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>22</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="6" t="s">
+        <v>10</v>
+      </c>
+      <c r="D7" s="8">
+        <v>69</v>
+      </c>
+      <c r="E7" s="4"/>
+    </row>
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A8" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B8" s="8">
+        <v>9999</v>
+      </c>
+      <c r="C8" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D8" s="8">
+        <v>13</v>
+      </c>
+      <c r="E8" s="8"/>
+    </row>
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A9" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B9" s="8"/>
+      <c r="C9" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D9" s="8">
+        <v>13</v>
+      </c>
+      <c r="E9" s="8"/>
+    </row>
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A10" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B10" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="6" t="s">
+        <v>71</v>
+      </c>
+      <c r="D10" s="8">
+        <v>13</v>
+      </c>
+      <c r="E10" s="8"/>
+    </row>
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A11" s="4" t="s">
+        <v>24</v>
+      </c>
+      <c r="B11" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="6" t="s">
+        <v>72</v>
+      </c>
+      <c r="D11" s="8">
+        <v>13</v>
+      </c>
+      <c r="E11" s="8"/>
+    </row>
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A12" s="4" t="s">
+        <v>69</v>
+      </c>
+      <c r="B12" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="6" t="s">
+        <v>73</v>
+      </c>
+      <c r="D12" s="8">
+        <v>13</v>
+      </c>
+      <c r="E12" s="8"/>
+    </row>
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A13" s="4" t="s">
+        <v>70</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="6" t="s">
+        <v>74</v>
+      </c>
+      <c r="D13" s="8">
+        <v>13</v>
+      </c>
+      <c r="E13" s="8"/>
+    </row>
+    <row r="14" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A14" s="4" t="s">
+        <v>27</v>
+      </c>
+      <c r="B14" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="6" t="s">
+        <v>75</v>
+      </c>
+      <c r="D14" s="8">
+        <v>13</v>
+      </c>
+      <c r="E14" s="8"/>
+    </row>
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A15" s="4" t="s">
+        <v>28</v>
+      </c>
+      <c r="B15" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="6" t="s">
+        <v>76</v>
+      </c>
+      <c r="D15" s="8">
+        <v>13</v>
+      </c>
+      <c r="E15" s="8"/>
+    </row>
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A16" s="4" t="s">
+        <v>29</v>
+      </c>
+      <c r="B16" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="6" t="s">
+        <v>77</v>
+      </c>
+      <c r="D16" s="8">
+        <v>13</v>
+      </c>
+      <c r="E16" s="8"/>
+    </row>
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A17" s="4" t="s">
+        <v>79</v>
+      </c>
+      <c r="B17" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D17" s="8">
+        <v>13</v>
+      </c>
+      <c r="E17" s="8"/>
+    </row>
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A18" s="4" t="s">
+        <v>80</v>
+      </c>
+      <c r="B18" s="8"/>
+      <c r="C18" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D18" s="9">
+        <v>9999</v>
+      </c>
+      <c r="E18" s="8"/>
+    </row>
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A19" s="4" t="s">
+        <v>81</v>
+      </c>
+      <c r="B19" s="8"/>
+      <c r="C19" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D19" s="8"/>
+      <c r="E19" s="8"/>
+    </row>
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A20" s="10" t="s">
+        <v>78</v>
+      </c>
+      <c r="B20" s="8"/>
+      <c r="C20" s="6" t="s">
+        <v>68</v>
+      </c>
+      <c r="D20" s="8">
+        <v>1</v>
+      </c>
+      <c r="E20" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F7D523-B9EA-2E4C-8630-43530090C6B3}">
   <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C1" sqref="C1:C7"/>
+      <selection activeCell="B8" sqref="B8:B15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -738,7 +1291,7 @@
         <v>4</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -815,7 +1368,7 @@
         <v>16</v>
       </c>
       <c r="C8" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -826,7 +1379,7 @@
         <v>62812</v>
       </c>
       <c r="C9" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.2">
@@ -837,7 +1390,7 @@
         <v>11</v>
       </c>
       <c r="C10" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.2">
@@ -848,7 +1401,7 @@
         <v>12</v>
       </c>
       <c r="C11" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.2">
@@ -859,7 +1412,7 @@
         <v>13</v>
       </c>
       <c r="C12" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.2">
@@ -870,7 +1423,7 @@
         <v>14</v>
       </c>
       <c r="C13" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="14" spans="1:3" x14ac:dyDescent="0.2">
@@ -881,7 +1434,7 @@
         <v>15</v>
       </c>
       <c r="C14" s="8" t="s">
-        <v>47</v>
+        <v>46</v>
       </c>
     </row>
     <row r="15" spans="1:3" x14ac:dyDescent="0.2">
@@ -890,7 +1443,7 @@
       </c>
       <c r="B15" s="6"/>
       <c r="C15" s="8" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
     </row>
   </sheetData>
@@ -898,7 +1451,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C10451-AC0E-B349-9A91-8F728BB33548}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -920,7 +1473,7 @@
         <v>31</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -996,8 +1549,8 @@
       <c r="B8" s="6" t="s">
         <v>38</v>
       </c>
-      <c r="C8" s="10" t="s">
-        <v>51</v>
+      <c r="C8" s="9" t="s">
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.2">
@@ -1005,8 +1558,8 @@
         <v>40</v>
       </c>
       <c r="B9" s="6"/>
-      <c r="C9" s="10" t="s">
-        <v>50</v>
+      <c r="C9" s="9" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>
@@ -1014,12 +1567,12 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B9D47F-9068-F44D-8E45-59D4A0B7482C}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1036,7 +1589,7 @@
         <v>41</v>
       </c>
       <c r="C1" s="7" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.2">
@@ -1047,7 +1600,7 @@
         <v>32</v>
       </c>
       <c r="C2" s="8" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.2">
@@ -1058,7 +1611,7 @@
         <v>33</v>
       </c>
       <c r="C3" s="8" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.2">
@@ -1067,7 +1620,7 @@
       </c>
       <c r="B4" s="4"/>
       <c r="C4" s="8" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
update create transaction remote service
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D3E99BF8-66CD-D646-B0F7-9638813B5ABE}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{46A56878-D9CF-4140-9787-9D69667B19A1}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="2" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" activeTab="3" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Recent Number" sheetId="2" r:id="rId1"/>
@@ -39,7 +39,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="194" uniqueCount="83">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="96">
   <si>
     <t>true</t>
   </si>
@@ -288,6 +288,45 @@
   </si>
   <si>
     <t>"number":"081252161795","provider":{"id":2,"name":"Telkomsel","image":"https://res.cloudinary.com/alvark/image/upload/v1592209103/danapulsa/Telkomsel_Logo_eviigt_nbbrjv.png"}</t>
+  </si>
+  <si>
+    <t>087735571982</t>
+  </si>
+  <si>
+    <t>089962192444</t>
+  </si>
+  <si>
+    <t>085655619187</t>
+  </si>
+  <si>
+    <t>0881025984984</t>
+  </si>
+  <si>
+    <t>083124211047</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"083124211047","catalog":{"id":69,"provider":{"id":6,"name":"Axis","image":"https://res.cloudinary.com/alvark/image/upload/v1592209102/danapulsa/Axis_logo_2015_fjybli_kgwzd1.png"},"value":5000,"price":6000}</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"0881025984984","catalog":{"id":58,"provider":{"id":5,"name":"Smartfren","image":"https://res.cloudinary.com/alvark/image/upload/v1592209103/danapulsa/Smartfren__282019_29_k5icie_grwdpg.png"},"value":5000,"price":5400}</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"085655619187","catalog":{"id":44,"provider":{"id":4,"name":"Indosat","image":"https://res.cloudinary.com/alvark/image/upload/v1592209102/danapulsa/Indosat_Ooredoo_logo_wcpr2o_nqcou3.png"},"value":10000,"price":11500}</t>
+  </si>
+  <si>
+    <t>selected catalog is not available for this phone’s provider</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"087735571982","catalog":{"id":1,"provider":{"id":1,"name":"XL","image":"https://res.cloudinary.com/alvark/image/upload/v1592209102/danapulsa/20180111100558_21XL_logo_2016_kyu40w_vkqgnc.png"},"value":5000,"price":6000}</t>
+  </si>
+  <si>
+    <t>catalog not found</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"089962192444","catalog":{"id":26,"provider":{"id":3,"name":"Tri","image":"https://res.cloudinary.com/alvark/image/upload/v1592209103/danapulsa/3-brand_cawkwp_pbjnni.png"},"value":1000,"price":1200}</t>
+  </si>
+  <si>
+    <t>unknown user</t>
   </si>
 </sst>
 </file>
@@ -899,7 +938,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{48440631-96CF-C448-B015-D93981B323AB}">
   <dimension ref="A1:C4"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="C34" sqref="C34"/>
     </sheetView>
   </sheetViews>
@@ -960,8 +999,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A5EF4B-A648-C44F-8302-8A78460D835D}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G18" sqref="G18"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="E26" sqref="E26"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -970,6 +1009,7 @@
     <col min="2" max="2" width="6.1640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="15.1640625" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="8.6640625" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="212.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:5" x14ac:dyDescent="0.2">
@@ -997,12 +1037,14 @@
         <v>0</v>
       </c>
       <c r="C2" s="6" t="s">
-        <v>5</v>
+        <v>83</v>
       </c>
       <c r="D2" s="8">
         <v>1</v>
       </c>
-      <c r="E2" s="8"/>
+      <c r="E2" s="8" t="s">
+        <v>92</v>
+      </c>
     </row>
     <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" s="4" t="s">
@@ -1017,7 +1059,9 @@
       <c r="D3" s="8">
         <v>13</v>
       </c>
-      <c r="E3" s="8"/>
+      <c r="E3" s="8" t="s">
+        <v>55</v>
+      </c>
     </row>
     <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -1027,12 +1071,14 @@
         <v>0</v>
       </c>
       <c r="C4" s="6" t="s">
-        <v>7</v>
+        <v>84</v>
       </c>
       <c r="D4" s="8">
         <v>26</v>
       </c>
-      <c r="E4" s="8"/>
+      <c r="E4" s="8" t="s">
+        <v>94</v>
+      </c>
     </row>
     <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" s="4" t="s">
@@ -1042,12 +1088,14 @@
         <v>0</v>
       </c>
       <c r="C5" s="6" t="s">
-        <v>8</v>
+        <v>85</v>
       </c>
       <c r="D5" s="8">
         <v>44</v>
       </c>
-      <c r="E5" s="8"/>
+      <c r="E5" s="8" t="s">
+        <v>90</v>
+      </c>
     </row>
     <row r="6" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A6" s="4" t="s">
@@ -1057,12 +1105,14 @@
         <v>0</v>
       </c>
       <c r="C6" s="6" t="s">
-        <v>9</v>
+        <v>86</v>
       </c>
       <c r="D6" s="8">
         <v>58</v>
       </c>
-      <c r="E6" s="4"/>
+      <c r="E6" s="4" t="s">
+        <v>89</v>
+      </c>
     </row>
     <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" s="4" t="s">
@@ -1072,12 +1122,14 @@
         <v>0</v>
       </c>
       <c r="C7" s="6" t="s">
-        <v>10</v>
+        <v>87</v>
       </c>
       <c r="D7" s="8">
         <v>69</v>
       </c>
-      <c r="E7" s="4"/>
+      <c r="E7" s="4" t="s">
+        <v>88</v>
+      </c>
     </row>
     <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" s="4" t="s">
@@ -1092,7 +1144,9 @@
       <c r="D8" s="8">
         <v>13</v>
       </c>
-      <c r="E8" s="8"/>
+      <c r="E8" s="8" t="s">
+        <v>95</v>
+      </c>
     </row>
     <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" s="4" t="s">
@@ -1105,7 +1159,9 @@
       <c r="D9" s="8">
         <v>13</v>
       </c>
-      <c r="E9" s="8"/>
+      <c r="E9" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" s="4" t="s">
@@ -1120,7 +1176,9 @@
       <c r="D10" s="8">
         <v>13</v>
       </c>
-      <c r="E10" s="8"/>
+      <c r="E10" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" s="4" t="s">
@@ -1135,7 +1193,9 @@
       <c r="D11" s="8">
         <v>13</v>
       </c>
-      <c r="E11" s="8"/>
+      <c r="E11" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" s="4" t="s">
@@ -1150,7 +1210,9 @@
       <c r="D12" s="8">
         <v>13</v>
       </c>
-      <c r="E12" s="8"/>
+      <c r="E12" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" s="4" t="s">
@@ -1165,7 +1227,9 @@
       <c r="D13" s="8">
         <v>13</v>
       </c>
-      <c r="E13" s="8"/>
+      <c r="E13" s="8" t="s">
+        <v>45</v>
+      </c>
     </row>
     <row r="14" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A14" s="4" t="s">
@@ -1180,7 +1244,9 @@
       <c r="D14" s="8">
         <v>13</v>
       </c>
-      <c r="E14" s="8"/>
+      <c r="E14" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" s="4" t="s">
@@ -1195,7 +1261,9 @@
       <c r="D15" s="8">
         <v>13</v>
       </c>
-      <c r="E15" s="8"/>
+      <c r="E15" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" s="4" t="s">
@@ -1210,7 +1278,9 @@
       <c r="D16" s="8">
         <v>13</v>
       </c>
-      <c r="E16" s="8"/>
+      <c r="E16" s="8" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" s="4" t="s">
@@ -1219,50 +1289,62 @@
       <c r="B17" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="C17" s="6" t="s">
-        <v>68</v>
-      </c>
+      <c r="C17" s="6"/>
       <c r="D17" s="8">
         <v>13</v>
       </c>
-      <c r="E17" s="8"/>
+      <c r="E17" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" s="4" t="s">
         <v>80</v>
       </c>
-      <c r="B18" s="8"/>
+      <c r="B18" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C18" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D18" s="9">
         <v>9999</v>
       </c>
-      <c r="E18" s="8"/>
+      <c r="E18" s="8" t="s">
+        <v>93</v>
+      </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" s="4" t="s">
         <v>81</v>
       </c>
-      <c r="B19" s="8"/>
+      <c r="B19" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C19" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D19" s="8"/>
-      <c r="E19" s="8"/>
+      <c r="E19" s="8" t="s">
+        <v>48</v>
+      </c>
     </row>
     <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" s="10" t="s">
         <v>78</v>
       </c>
-      <c r="B20" s="8"/>
+      <c r="B20" s="1" t="s">
+        <v>0</v>
+      </c>
       <c r="C20" s="6" t="s">
         <v>68</v>
       </c>
       <c r="D20" s="8">
         <v>1</v>
       </c>
-      <c r="E20" s="8"/>
+      <c r="E20" s="8" t="s">
+        <v>91</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update history and vouchers
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -8,18 +8,20 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B7AA4D4A-1559-674E-870E-752063C1482E}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD899E9-A422-BC46-97CC-DCFC3DEBA1EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="3" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Recent Number" sheetId="2" r:id="rId1"/>
     <sheet name="Get Transaction By Id By UserId" sheetId="7" r:id="rId2"/>
     <sheet name="Get Transaction By ID" sheetId="3" r:id="rId3"/>
     <sheet name="Create Transaction" sheetId="8" r:id="rId4"/>
-    <sheet name="Get All Catalog" sheetId="4" r:id="rId5"/>
-    <sheet name="Get Provider By ID" sheetId="5" r:id="rId6"/>
-    <sheet name="Get Payment Method Name By ID" sheetId="6" r:id="rId7"/>
+    <sheet name="Get History in Progress" sheetId="9" r:id="rId5"/>
+    <sheet name="Get History Completed" sheetId="10" r:id="rId6"/>
+    <sheet name="Get All Catalog" sheetId="4" r:id="rId7"/>
+    <sheet name="Get Provider By ID" sheetId="5" r:id="rId8"/>
+    <sheet name="Get Payment Method Name By ID" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -39,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="215" uniqueCount="96">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="104">
   <si>
     <t>true</t>
   </si>
@@ -327,6 +329,30 @@
   </si>
   <si>
     <t>unknown user</t>
+  </si>
+  <si>
+    <t>page</t>
+  </si>
+  <si>
+    <t>Undefined user id</t>
+  </si>
+  <si>
+    <t>Empty string user id</t>
+  </si>
+  <si>
+    <t>Undefined page</t>
+  </si>
+  <si>
+    <t>Empty string page</t>
+  </si>
+  <si>
+    <t>Valid user id and page (no history)</t>
+  </si>
+  <si>
+    <t>Valid user id and page (below 10 history)</t>
+  </si>
+  <si>
+    <t>Valid user id and page (more than 10 history)</t>
   </si>
 </sst>
 </file>
@@ -396,7 +422,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="13">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -412,6 +438,10 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="left"/>
+    </xf>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -729,7 +759,7 @@
   <dimension ref="A1:C6"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A10" sqref="A10"/>
+      <selection activeCell="B34" sqref="B34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -812,7 +842,7 @@
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D12" sqref="D12"/>
+      <selection activeCell="D31" sqref="D31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -939,7 +969,7 @@
   <dimension ref="A1:C4"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="C34" sqref="C34"/>
+      <selection activeCell="C35" sqref="C35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -999,7 +1029,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9A5EF4B-A648-C44F-8302-8A78460D835D}">
   <dimension ref="A1:E20"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="E32" sqref="E32"/>
     </sheetView>
   </sheetViews>
@@ -1352,11 +1382,281 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13A6D6E-685E-0A43-9E10-D43823A45D9B}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="F28" sqref="F28"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="4" width="19.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9999</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E585D37-39C0-D544-BC90-55ADE72DC8E5}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="I33" sqref="I33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="3" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="11" t="s">
+        <v>96</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>101</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1">
+        <v>1</v>
+      </c>
+      <c r="D2" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1">
+        <v>1</v>
+      </c>
+      <c r="D3" s="8"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C4" s="1">
+        <v>1</v>
+      </c>
+      <c r="D4" s="8"/>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="1" t="s">
+        <v>103</v>
+      </c>
+      <c r="B5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C5" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="D5" s="8"/>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="1" t="s">
+        <v>97</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C6" s="1">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="12" t="s">
+        <v>98</v>
+      </c>
+      <c r="B7" s="6"/>
+      <c r="C7" s="1">
+        <v>1</v>
+      </c>
+      <c r="D7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="1" t="s">
+        <v>99</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="1">
+        <v>9999</v>
+      </c>
+      <c r="D8" s="8" t="s">
+        <v>56</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="1" t="s">
+        <v>100</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1"/>
+      <c r="D9" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F7D523-B9EA-2E4C-8630-43530090C6B3}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="G29" sqref="G29"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1533,7 +1833,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C10451-AC0E-B349-9A91-8F728BB33548}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1649,7 +1949,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B9D47F-9068-F44D-8E45-59D4A0B7482C}">
   <dimension ref="A1:C4"/>
   <sheetViews>

</xml_diff>

<commit_message>
update code for mobile domain
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6FD899E9-A422-BC46-97CC-DCFC3DEBA1EB}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC18D01-4C56-A349-B7FE-02A3273BD216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="6" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Recent Number" sheetId="2" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="265" uniqueCount="104">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="110">
   <si>
     <t>true</t>
   </si>
@@ -353,6 +353,24 @@
   </si>
   <si>
     <t>Valid user id and page (more than 10 history)</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"081252930398","price":15000,"voucher":0,"status":"COMPLETED"</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"0812521617910","price":15000,"voucher":0,"status":"COMPLETED"</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"081252161790","price":15000,"voucher":0,"status":"COMPLETED"</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"081252930398","price":15000,"voucher":0,"status":"WAITING"</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"0812521617910","price":15000,"voucher":0,"status":"WAITING"</t>
+  </si>
+  <si>
+    <t>"phoneNumber":"081252161790","price":15000,"voucher":0,"status":"WAITING"</t>
   </si>
 </sst>
 </file>
@@ -1385,14 +1403,15 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13A6D6E-685E-0A43-9E10-D43823A45D9B}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="F28" sqref="F28"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="36.6640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="69.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1433,7 +1452,9 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="8" t="s">
+        <v>107</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1445,7 +1466,9 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="8" t="s">
+        <v>108</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1457,7 +1480,9 @@
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>109</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1521,13 +1546,13 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="I33" sqref="I33"/>
+      <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="35.1640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="19.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="104.83203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1568,7 +1593,9 @@
       <c r="C3" s="1">
         <v>1</v>
       </c>
-      <c r="D3" s="8"/>
+      <c r="D3" s="8" t="s">
+        <v>104</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
@@ -1580,7 +1607,9 @@
       <c r="C4" s="1">
         <v>1</v>
       </c>
-      <c r="D4" s="8"/>
+      <c r="D4" s="8" t="s">
+        <v>105</v>
+      </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
@@ -1592,7 +1621,9 @@
       <c r="C5" s="1" t="s">
         <v>33</v>
       </c>
-      <c r="D5" s="8"/>
+      <c r="D5" s="8" t="s">
+        <v>106</v>
+      </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
@@ -1655,7 +1686,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F7D523-B9EA-2E4C-8630-43530090C6B3}">
   <dimension ref="A1:C15"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="K33" sqref="K33"/>
     </sheetView>
   </sheetViews>

</xml_diff>

<commit_message>
update cancel order code
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FFC18D01-4C56-A349-B7FE-02A3273BD216}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9280FC-A0B2-7148-9F86-D7682C7E9CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" activeTab="4" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="5" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Recent Number" sheetId="2" r:id="rId1"/>
@@ -18,10 +18,12 @@
     <sheet name="Get Transaction By ID" sheetId="3" r:id="rId3"/>
     <sheet name="Create Transaction" sheetId="8" r:id="rId4"/>
     <sheet name="Get History in Progress" sheetId="9" r:id="rId5"/>
-    <sheet name="Get History Completed" sheetId="10" r:id="rId6"/>
-    <sheet name="Get All Catalog" sheetId="4" r:id="rId7"/>
-    <sheet name="Get Provider By ID" sheetId="5" r:id="rId8"/>
-    <sheet name="Get Payment Method Name By ID" sheetId="6" r:id="rId9"/>
+    <sheet name="Cancel" sheetId="11" r:id="rId6"/>
+    <sheet name="Get History Completed" sheetId="10" r:id="rId7"/>
+    <sheet name="Get All Catalog" sheetId="4" r:id="rId8"/>
+    <sheet name="Get Provider By ID" sheetId="5" r:id="rId9"/>
+    <sheet name="Get Payment Method Name By ID" sheetId="6" r:id="rId10"/>
+    <sheet name="Pay" sheetId="12" r:id="rId11"/>
   </sheets>
   <calcPr calcId="181029"/>
   <extLst>
@@ -41,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="271" uniqueCount="110">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="111">
   <si>
     <t>true</t>
   </si>
@@ -371,6 +373,9 @@
   </si>
   <si>
     <t>"phoneNumber":"081252161790","price":15000,"voucher":0,"status":"WAITING"</t>
+  </si>
+  <si>
+    <t>Transaction already completed</t>
   </si>
 </sst>
 </file>
@@ -855,12 +860,85 @@
 </worksheet>
 </file>
 
+<file path=xl/worksheets/sheet10.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B9D47F-9068-F44D-8E45-59D4A0B7482C}">
+  <dimension ref="A1:C4"/>
+  <sheetViews>
+    <sheetView workbookViewId="0">
+      <selection activeCell="B23" sqref="B23"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>41</v>
+      </c>
+      <c r="C1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A2" s="8" t="s">
+        <v>42</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>32</v>
+      </c>
+      <c r="C2" s="8" t="s">
+        <v>50</v>
+      </c>
+    </row>
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A3" s="8" t="s">
+        <v>39</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>33</v>
+      </c>
+      <c r="C3" s="8" t="s">
+        <v>51</v>
+      </c>
+    </row>
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A4" s="8" t="s">
+        <v>40</v>
+      </c>
+      <c r="B4" s="4"/>
+      <c r="C4" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0043022C-EAA4-0B4E-B994-33ABFD3F9678}">
+  <dimension ref="A1"/>
+  <sheetViews>
+    <sheetView workbookViewId="0"/>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <sheetData/>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1B2C1876-3DA3-8644-B3D6-CD5FFA8B91C1}">
   <dimension ref="A1:D8"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D31" sqref="D31"/>
+      <selection sqref="A1:D8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1403,7 +1481,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D13A6D6E-685E-0A43-9E10-D43823A45D9B}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="D6" sqref="D6"/>
     </sheetView>
   </sheetViews>
@@ -1542,6 +1620,141 @@
 </file>
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6DE50B-2548-AF4E-A530-F44ACAB8D61E}">
+  <dimension ref="A1:D9"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="B19" sqref="B19"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="223.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A1" s="7" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="3" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="3" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="7" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A2" s="4" t="s">
+        <v>58</v>
+      </c>
+      <c r="B2" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D2" s="4" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A3" s="4" t="s">
+        <v>59</v>
+      </c>
+      <c r="B3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="4"/>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A4" s="4" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="8" t="s">
+        <v>95</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A5" s="4" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="4"/>
+      <c r="C5" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A6" s="4" t="s">
+        <v>63</v>
+      </c>
+      <c r="B6" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="1" t="s">
+        <v>1</v>
+      </c>
+      <c r="D6" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A7" s="4" t="s">
+        <v>64</v>
+      </c>
+      <c r="B7" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="8"/>
+      <c r="D7" s="8" t="s">
+        <v>48</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A8" s="10" t="s">
+        <v>62</v>
+      </c>
+      <c r="B8" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="8"/>
+      <c r="D8" s="8" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+      <c r="A9" s="10" t="s">
+        <v>110</v>
+      </c>
+      <c r="B9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="D9" s="8"/>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{4E585D37-39C0-D544-BC90-55ADE72DC8E5}">
   <dimension ref="A1:D9"/>
   <sheetViews>
@@ -1682,7 +1895,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{59F7D523-B9EA-2E4C-8630-43530090C6B3}">
   <dimension ref="A1:C15"/>
   <sheetViews>
@@ -1864,7 +2077,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B9C10451-AC0E-B349-9A91-8F728BB33548}">
   <dimension ref="A1:C9"/>
   <sheetViews>
@@ -1978,65 +2191,4 @@
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
-</file>
-
-<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{E8B9D47F-9068-F44D-8E45-59D4A0B7482C}">
-  <dimension ref="A1:C4"/>
-  <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B23" sqref="B23"/>
-    </sheetView>
-  </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <cols>
-    <col min="1" max="1" width="11.83203125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="19.5" bestFit="1" customWidth="1"/>
-  </cols>
-  <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A1" s="7" t="s">
-        <v>43</v>
-      </c>
-      <c r="B1" s="3" t="s">
-        <v>41</v>
-      </c>
-      <c r="C1" s="7" t="s">
-        <v>44</v>
-      </c>
-    </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" s="8" t="s">
-        <v>42</v>
-      </c>
-      <c r="B2" s="1" t="s">
-        <v>32</v>
-      </c>
-      <c r="C2" s="8" t="s">
-        <v>50</v>
-      </c>
-    </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" s="8" t="s">
-        <v>39</v>
-      </c>
-      <c r="B3" s="1" t="s">
-        <v>33</v>
-      </c>
-      <c r="C3" s="8" t="s">
-        <v>51</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" s="8" t="s">
-        <v>40</v>
-      </c>
-      <c r="B4" s="4"/>
-      <c r="C4" s="8" t="s">
-        <v>48</v>
-      </c>
-    </row>
-  </sheetData>
-  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-</worksheet>
 </file>
</xml_diff>

<commit_message>
update get voucher recommendation code
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FA9280FC-A0B2-7148-9F86-D7682C7E9CA6}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EBDC0B-F45B-4344-8A99-7E1072A07E85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="5" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" firstSheet="2" activeTab="5" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Recent Number" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="302" uniqueCount="111">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="113">
   <si>
     <t>true</t>
   </si>
@@ -376,6 +376,12 @@
   </si>
   <si>
     <t>Transaction already completed</t>
+  </si>
+  <si>
+    <t>can't cancel completed transaction</t>
+  </si>
+  <si>
+    <t>"method":"WALLET","phoneNumber":"081252930398","catalog":{"id":13,"provider":{"id":2,"name":"Telkomsel","image":"https://res.cloudinary.com/alvark/image/upload/v1592209103/danapulsa/Telkomsel_Logo_eviigt_nbbrjv.png"},"value":15000,"price":15000},"status":"CANCELED"</t>
   </si>
 </sst>
 </file>
@@ -1624,13 +1630,13 @@
   <dimension ref="A1:D9"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="B19" sqref="B19"/>
+      <selection activeCell="D17" sqref="D17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="26.83203125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="223.83203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="242.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" x14ac:dyDescent="0.2">
@@ -1671,7 +1677,9 @@
       <c r="C3" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D3" s="4"/>
+      <c r="D3" s="4" t="s">
+        <v>112</v>
+      </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" s="4" t="s">
@@ -1747,7 +1755,9 @@
       <c r="C9" s="1" t="s">
         <v>0</v>
       </c>
-      <c r="D9" s="8"/>
+      <c r="D9" s="8" t="s">
+        <v>111</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
update remote service payment code
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{55EBDC0B-F45B-4344-8A99-7E1072A07E85}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A17EB439-5D07-3741-AC10-0ADF42F2F577}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="28800" windowHeight="16500" firstSheet="2" activeTab="5" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="2" activeTab="10" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
   <sheets>
     <sheet name="Get Recent Number" sheetId="2" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="304" uniqueCount="113">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="395" uniqueCount="127">
   <si>
     <t>true</t>
   </si>
@@ -382,13 +382,55 @@
   </si>
   <si>
     <t>"method":"WALLET","phoneNumber":"081252930398","catalog":{"id":13,"provider":{"id":2,"name":"Telkomsel","image":"https://res.cloudinary.com/alvark/image/upload/v1592209103/danapulsa/Telkomsel_Logo_eviigt_nbbrjv.png"},"value":15000,"price":15000},"status":"CANCELED"</t>
+  </si>
+  <si>
+    <t>paymentMethodId</t>
+  </si>
+  <si>
+    <t>voucherId</t>
+  </si>
+  <si>
+    <t>Valid parameters cashback</t>
+  </si>
+  <si>
+    <t>Valid parameters discount</t>
+  </si>
+  <si>
+    <t>Not enough balance</t>
+  </si>
+  <si>
+    <t>Transaction already canceled</t>
+  </si>
+  <si>
+    <t>Transaction already expired</t>
+  </si>
+  <si>
+    <t>Undefined payment method ID</t>
+  </si>
+  <si>
+    <t>Empty string payment method ID</t>
+  </si>
+  <si>
+    <t>Undefined voucher id</t>
+  </si>
+  <si>
+    <t>Empty string voucher id</t>
+  </si>
+  <si>
+    <t>Voucher not available for the transaction</t>
+  </si>
+  <si>
+    <t>Voucher already used</t>
+  </si>
+  <si>
+    <t>Voucher expired</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <fonts count="3" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
       <color theme="1"/>
@@ -398,6 +440,13 @@
     </font>
     <font>
       <sz val="11"/>
+      <color rgb="FF000000"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="12"/>
       <color rgb="FF000000"/>
       <name val="Calibri"/>
       <family val="2"/>
@@ -451,7 +500,7 @@
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="13">
+  <cellXfs count="19">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -471,6 +520,12 @@
     <xf numFmtId="49" fontId="1" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="49" fontId="2" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="2" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -929,12 +984,356 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0043022C-EAA4-0B4E-B994-33ABFD3F9678}">
-  <dimension ref="A1"/>
+  <dimension ref="A1:F19"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H8" sqref="H8"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
-  <sheetData/>
+  <cols>
+    <col min="1" max="1" width="32.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="5.83203125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="11.33203125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.33203125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="8.83203125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A1" s="14" t="s">
+        <v>43</v>
+      </c>
+      <c r="B1" s="15" t="s">
+        <v>3</v>
+      </c>
+      <c r="C1" s="15" t="s">
+        <v>2</v>
+      </c>
+      <c r="D1" s="15" t="s">
+        <v>113</v>
+      </c>
+      <c r="E1" s="15" t="s">
+        <v>114</v>
+      </c>
+      <c r="F1" s="14" t="s">
+        <v>44</v>
+      </c>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A2" s="16" t="s">
+        <v>115</v>
+      </c>
+      <c r="B2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C2" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E2" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="16"/>
+    </row>
+    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A3" s="16" t="s">
+        <v>116</v>
+      </c>
+      <c r="B3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C3" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D3" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E3" s="13" t="s">
+        <v>38</v>
+      </c>
+      <c r="F3" s="16"/>
+    </row>
+    <row r="4" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A4" s="16" t="s">
+        <v>60</v>
+      </c>
+      <c r="B4" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="C4" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E4" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F4" s="17"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" s="16" t="s">
+        <v>61</v>
+      </c>
+      <c r="B5" s="16"/>
+      <c r="C5" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E5" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F5" s="17"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A6" s="16" t="s">
+        <v>117</v>
+      </c>
+      <c r="B6" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C6" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E6" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F6" s="17"/>
+    </row>
+    <row r="7" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A7" s="16" t="s">
+        <v>63</v>
+      </c>
+      <c r="B7" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C7" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="D7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E7" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F7" s="17"/>
+    </row>
+    <row r="8" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A8" s="16" t="s">
+        <v>64</v>
+      </c>
+      <c r="B8" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C8" s="17"/>
+      <c r="D8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E8" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F8" s="17"/>
+    </row>
+    <row r="9" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A9" s="18" t="s">
+        <v>62</v>
+      </c>
+      <c r="B9" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C9" s="17"/>
+      <c r="D9" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E9" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F9" s="17"/>
+    </row>
+    <row r="10" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A10" s="18" t="s">
+        <v>110</v>
+      </c>
+      <c r="B10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C10" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E10" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F10" s="17"/>
+    </row>
+    <row r="11" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A11" s="18" t="s">
+        <v>118</v>
+      </c>
+      <c r="B11" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C11" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E11" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F11" s="17"/>
+    </row>
+    <row r="12" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A12" s="13" t="s">
+        <v>119</v>
+      </c>
+      <c r="B12" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C12" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E12" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F12" s="17"/>
+    </row>
+    <row r="13" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A13" s="18" t="s">
+        <v>120</v>
+      </c>
+      <c r="B13" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C13" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D13" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="E13" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F13" s="17"/>
+    </row>
+    <row r="14" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A14" s="18" t="s">
+        <v>121</v>
+      </c>
+      <c r="B14" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C14" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D14" s="13"/>
+      <c r="E14" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="F14" s="17"/>
+    </row>
+    <row r="15" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A15" s="13" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C15" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D15" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E15" s="13" t="s">
+        <v>1</v>
+      </c>
+      <c r="F15" s="17"/>
+    </row>
+    <row r="16" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A16" s="13" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C16" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D16" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E16" s="13"/>
+      <c r="F16" s="17"/>
+    </row>
+    <row r="17" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A17" s="13" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C17" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D17" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E17" s="13" t="s">
+        <v>33</v>
+      </c>
+      <c r="F17" s="17"/>
+    </row>
+    <row r="18" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A18" s="13" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C18" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D18" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E18" s="13" t="s">
+        <v>34</v>
+      </c>
+      <c r="F18" s="17"/>
+    </row>
+    <row r="19" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A19" s="13" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="C19" s="13" t="s">
+        <v>0</v>
+      </c>
+      <c r="D19" s="13" t="s">
+        <v>32</v>
+      </c>
+      <c r="E19" s="13" t="s">
+        <v>35</v>
+      </c>
+      <c r="F19" s="17"/>
+    </row>
+  </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
@@ -1629,8 +2028,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9D6DE50B-2548-AF4E-A530-F44ACAB8D61E}">
   <dimension ref="A1:D9"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D17" sqref="D17"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:D9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>

<commit_message>
update connection remote mysql promotion
</commit_message>
<xml_diff>
--- a/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
+++ b/src/test/java/remoteService/order/RemoteServiceOrderTestData.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/romadonz/Documents/Zanuar/DANA/Hands On Project/DANA Pulsa/Automation Testing/DanaPulsaAutomationTest/src/test/java/remoteService/order/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AB9E3AF-4CCE-454B-A5D5-3AE058B9E681}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A3C46F71-B1F0-204D-99C0-7FB9229C71DF}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" firstSheet="3" activeTab="10" xr2:uid="{0BFCFD56-4938-304E-8F8D-A74A800CA122}"/>
   </bookViews>
@@ -44,7 +44,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="435" uniqueCount="135">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="431" uniqueCount="135">
   <si>
     <t>true</t>
   </si>
@@ -1010,10 +1010,10 @@
 
 <file path=xl/worksheets/sheet11.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{0043022C-EAA4-0B4E-B994-33ABFD3F9678}">
-  <dimension ref="A1:F3"/>
+  <dimension ref="A1:F2"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C17" sqref="C17"/>
+      <selection activeCell="F32" sqref="F32"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1048,7 +1048,7 @@
     </row>
     <row r="2" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A2" s="16" t="s">
-        <v>115</v>
+        <v>132</v>
       </c>
       <c r="B2" s="13" t="s">
         <v>0</v>
@@ -1060,27 +1060,11 @@
         <v>32</v>
       </c>
       <c r="E2" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="F2" s="16"/>
-    </row>
-    <row r="3" spans="1:6" x14ac:dyDescent="0.2">
-      <c r="A3" s="16" t="s">
-        <v>116</v>
-      </c>
-      <c r="B3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="C3" s="13" t="s">
-        <v>0</v>
-      </c>
-      <c r="D3" s="13" t="s">
-        <v>32</v>
-      </c>
-      <c r="E3" s="13" t="s">
-        <v>38</v>
-      </c>
-      <c r="F3" s="16"/>
+        <v>133</v>
+      </c>
+      <c r="F2" s="16" t="s">
+        <v>134</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -1092,7 +1076,7 @@
   <dimension ref="A1:F21"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A3" sqref="A3:F4"/>
+      <selection activeCell="F36" sqref="F36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>

</xml_diff>